<commit_message>
solo 2 decimales en excel de facturas
</commit_message>
<xml_diff>
--- a/FacturacionSW/FACTURAS.xlsx
+++ b/FacturacionSW/FACTURAS.xlsx
@@ -378,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -472,6 +472,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,8 +502,8 @@
       <xdr:rowOff>32648</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>464819</xdr:rowOff>
     </xdr:to>
@@ -824,7 +825,7 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,11 +957,11 @@
       <c r="E7" s="3"/>
       <c r="F7" s="4"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="3">
+      <c r="H7" s="37">
         <f t="shared" ref="H7:H33" si="0">+F7*G7/100</f>
         <v>0</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="37">
         <f>F7+H7</f>
         <v>0</v>
       </c>
@@ -973,11 +974,11 @@
       <c r="E8" s="3"/>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="3">
+      <c r="H8" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="37">
         <f t="shared" ref="I8:I33" si="1">F8+H8</f>
         <v>0</v>
       </c>
@@ -990,11 +991,11 @@
       <c r="E9" s="3"/>
       <c r="F9" s="4"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="3">
+      <c r="H9" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1007,11 +1008,11 @@
       <c r="E10" s="3"/>
       <c r="F10" s="4"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="3">
+      <c r="H10" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1024,11 +1025,11 @@
       <c r="E11" s="3"/>
       <c r="F11" s="4"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="3">
+      <c r="H11" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1041,11 +1042,11 @@
       <c r="E12" s="3"/>
       <c r="F12" s="4"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="3">
+      <c r="H12" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1058,11 +1059,11 @@
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="3">
+      <c r="H13" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1075,11 +1076,11 @@
       <c r="E14" s="3"/>
       <c r="F14" s="4"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="3">
+      <c r="H14" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1092,11 +1093,11 @@
       <c r="E15" s="3"/>
       <c r="F15" s="4"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="3">
+      <c r="H15" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1109,11 +1110,11 @@
       <c r="E16" s="3"/>
       <c r="F16" s="4"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="3">
+      <c r="H16" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1126,11 +1127,11 @@
       <c r="E17" s="3"/>
       <c r="F17" s="4"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="3">
+      <c r="H17" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1143,11 +1144,11 @@
       <c r="E18" s="3"/>
       <c r="F18" s="4"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="3">
+      <c r="H18" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1160,11 +1161,11 @@
       <c r="E19" s="3"/>
       <c r="F19" s="4"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="3">
+      <c r="H19" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1177,11 +1178,11 @@
       <c r="E20" s="3"/>
       <c r="F20" s="4"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="3">
+      <c r="H20" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1194,12 +1195,12 @@
       <c r="E21" s="3"/>
       <c r="F21" s="4"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="3">
-        <f>F21+H21</f>
+      <c r="H21" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="37">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1211,11 +1212,11 @@
       <c r="E22" s="3"/>
       <c r="F22" s="4"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="3">
+      <c r="H22" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1228,11 +1229,11 @@
       <c r="E23" s="3"/>
       <c r="F23" s="4"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="3">
+      <c r="H23" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1245,11 +1246,11 @@
       <c r="E24" s="3"/>
       <c r="F24" s="4"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I24" s="3">
+      <c r="H24" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1262,11 +1263,11 @@
       <c r="E25" s="3"/>
       <c r="F25" s="4"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="3">
+      <c r="H25" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1279,11 +1280,11 @@
       <c r="E26" s="3"/>
       <c r="F26" s="4"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="3">
+      <c r="H26" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1296,11 +1297,11 @@
       <c r="E27" s="3"/>
       <c r="F27" s="4"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I27" s="3">
+      <c r="H27" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1313,11 +1314,11 @@
       <c r="E28" s="3"/>
       <c r="F28" s="4"/>
       <c r="G28" s="5"/>
-      <c r="H28" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I28" s="3">
+      <c r="H28" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1330,11 +1331,11 @@
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
       <c r="G29" s="5"/>
-      <c r="H29" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I29" s="3">
+      <c r="H29" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1347,11 +1348,11 @@
       <c r="E30" s="3"/>
       <c r="F30" s="4"/>
       <c r="G30" s="5"/>
-      <c r="H30" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I30" s="3">
+      <c r="H30" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1364,11 +1365,11 @@
       <c r="E31" s="3"/>
       <c r="F31" s="4"/>
       <c r="G31" s="5"/>
-      <c r="H31" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I31" s="3">
+      <c r="H31" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1381,11 +1382,11 @@
       <c r="E32" s="3"/>
       <c r="F32" s="4"/>
       <c r="G32" s="5"/>
-      <c r="H32" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I32" s="3">
+      <c r="H32" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1398,11 +1399,11 @@
       <c r="E33" s="3"/>
       <c r="F33" s="4"/>
       <c r="G33" s="5"/>
-      <c r="H33" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I33" s="3">
+      <c r="H33" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>